<commit_message>
Se añade tax Ninguno.
</commit_message>
<xml_diff>
--- a/Registros.xlsx
+++ b/Registros.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmont\Documents\Funny\Python\Alegra\alegraApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmont\Documents\Some Code\Python\Alegra\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59142F14-8A53-4DAA-A2C9-E361DC21291A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F72D61-D31A-41BE-ADA3-A0D5D099703D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -852,7 +852,7 @@
   </sheetPr>
   <dimension ref="A1:RB29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
@@ -4207,7 +4207,9 @@
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
+      <c r="F7" s="39">
+        <v>0.05</v>
+      </c>
       <c r="G7" s="40" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Some refactor api: STABLE VERSION
</commit_message>
<xml_diff>
--- a/Registros.xlsx
+++ b/Registros.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ENVIABLES" sheetId="1" state="visible" r:id="rId1"/>
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -208,7 +208,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -597,20 +596,21 @@
   </sheetPr>
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="10.90625" customWidth="1" style="29" min="2" max="2"/>
-    <col width="17.26953125" customWidth="1" style="29" min="4" max="4"/>
-    <col width="14.453125" customWidth="1" style="29" min="5" max="5"/>
-    <col width="20.1796875" customWidth="1" style="29" min="7" max="7"/>
-    <col width="21.7265625" customWidth="1" style="29" min="8" max="8"/>
-    <col width="10.90625" customWidth="1" style="29" min="16" max="16"/>
-    <col width="15.26953125" customWidth="1" style="29" min="21" max="21"/>
-    <col width="10.90625" customWidth="1" style="29" min="23" max="23"/>
+    <col width="10.85546875" customWidth="1" min="2" max="2"/>
+    <col width="17.28515625" customWidth="1" min="4" max="4"/>
+    <col width="14.42578125" customWidth="1" min="5" max="5"/>
+    <col width="20.140625" customWidth="1" min="7" max="7"/>
+    <col width="21.7109375" customWidth="1" min="8" max="8"/>
+    <col width="10.85546875" customWidth="1" min="16" max="16"/>
+    <col width="16.85546875" customWidth="1" min="18" max="18"/>
+    <col width="15.28515625" customWidth="1" min="21" max="21"/>
+    <col width="10.85546875" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -781,7 +781,7 @@
       <c r="C3" s="12" t="n">
         <v>44366</v>
       </c>
-      <c r="D3" s="32" t="inlineStr">
+      <c r="D3" s="31" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="11" t="n"/>
-      <c r="H5" s="30" t="n"/>
+      <c r="H5" s="29" t="n"/>
       <c r="I5" s="15" t="n"/>
       <c r="J5" s="15" t="n"/>
       <c r="K5" s="9" t="n"/>
@@ -1036,7 +1036,7 @@
           <t>Samuel rendon</t>
         </is>
       </c>
-      <c r="H7" s="31" t="n">
+      <c r="H7" s="30" t="n">
         <v>3560832</v>
       </c>
       <c r="I7" s="15" t="inlineStr">
@@ -1113,7 +1113,7 @@
       <c r="E8" s="15" t="n"/>
       <c r="F8" s="11" t="n"/>
       <c r="G8" s="11" t="n"/>
-      <c r="H8" s="30" t="n"/>
+      <c r="H8" s="29" t="n"/>
       <c r="I8" s="14" t="n"/>
       <c r="J8" s="14" t="n"/>
       <c r="K8" s="9" t="n"/>
@@ -1207,7 +1207,7 @@
           <t>Samuel Rendon SAS</t>
         </is>
       </c>
-      <c r="H10" s="31" t="n">
+      <c r="H10" s="30" t="n">
         <v>901352563</v>
       </c>
       <c r="I10" s="15" t="inlineStr">

</xml_diff>

<commit_message>
Some changes, estate change for refactor.
</commit_message>
<xml_diff>
--- a/Registros.xlsx
+++ b/Registros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmont\Documents\Code\Projs\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5D848F-0CA1-4666-97EB-DEBD41A904AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F212BCCB-4AFB-48BD-BFED-E960991219A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENVIABLES" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>FECHA</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>pendiente</t>
+  </si>
+  <si>
+    <t>Cotizacion</t>
   </si>
 </sst>
 </file>
@@ -689,24 +692,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" customWidth="1"/>
-    <col min="8" max="8" width="21.7265625" customWidth="1"/>
-    <col min="16" max="16" width="10.81640625" customWidth="1"/>
-    <col min="18" max="18" width="16.81640625" customWidth="1"/>
-    <col min="21" max="21" width="15.26953125" customWidth="1"/>
-    <col min="23" max="23" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -786,7 +789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -814,7 +817,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>44366</v>
       </c>
@@ -893,7 +896,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -945,7 +948,7 @@
         <v>360000</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -995,7 +998,7 @@
         <v>72000</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
@@ -1023,7 +1026,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>44365</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1144,7 +1147,7 @@
         <v>360000</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
@@ -1172,7 +1175,7 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>44365</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>44365</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>27</v>
@@ -1249,10 +1252,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="X12" s="24"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H14" s="24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Refactor AlegraApp.bat to use app.py instead of lanzamiento.py
</commit_message>
<xml_diff>
--- a/Registros.xlsx
+++ b/Registros.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5190" yWindow="4245" windowWidth="21600" windowHeight="11235" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4320" yWindow="3720" windowWidth="21600" windowHeight="11235" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ENVIABLES" sheetId="1" state="visible" r:id="rId1"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -878,7 +878,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Cargado</t>
+          <t>Pendiente</t>
         </is>
       </c>
     </row>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>Cargado</t>
+          <t>Pendiente</t>
         </is>
       </c>
     </row>

</xml_diff>